<commit_message>
clear process ก่อน test
</commit_message>
<xml_diff>
--- a/XCustPr/doc/60-11-29/RD_INTERNAL_TEST_PLAN.xlsx
+++ b/XCustPr/doc/60-11-29/RD_INTERNAL_TEST_PLAN.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_ICE_2016\RD\00_PMO_Templates (13-May)\10-Planning\12-Project Plan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8964" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8970" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -225,21 +220,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -247,7 +242,7 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -387,15 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,7 +410,14 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -433,7 +426,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -720,64 +715,64 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.19921875" customWidth="1"/>
-    <col min="3" max="3" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.296875" customWidth="1"/>
-    <col min="5" max="5" width="17.3984375" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.19921875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="12"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="6">
@@ -788,7 +783,7 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I3" t="s">
@@ -796,13 +791,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="6">
@@ -813,7 +808,7 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I4" t="s">
@@ -821,13 +816,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="6">
@@ -838,7 +833,7 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I5" t="s">
@@ -846,13 +841,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="6">
@@ -867,7 +862,7 @@
       <c r="G6" s="6">
         <v>43073</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="I6" t="s">
@@ -875,13 +870,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="6">
@@ -896,7 +891,7 @@
       <c r="G7" s="6">
         <v>43075</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
@@ -904,13 +899,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="6">
@@ -927,28 +922,28 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>43076</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="8">
         <v>43076</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>43076</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>43076</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="12" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
@@ -956,13 +951,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="3">
@@ -971,18 +966,18 @@
       <c r="E10" s="3">
         <v>43077</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="3">
@@ -991,18 +986,18 @@
       <c r="E11" s="3">
         <v>43077</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="3">
@@ -1011,18 +1006,18 @@
       <c r="E12" s="3">
         <v>43077</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="20">
         <v>11</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="3">
@@ -1031,7 +1026,7 @@
       <c r="E13" s="3">
         <v>43075</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="11" t="s">
         <v>23</v>
       </c>
       <c r="I13" t="s">
@@ -1039,13 +1034,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="16">
         <v>12</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="3">
@@ -1054,18 +1049,18 @@
       <c r="E14" s="3">
         <v>43080</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="16">
         <v>13</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="19" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="3">
@@ -1074,18 +1069,18 @@
       <c r="E15" s="3">
         <v>43080</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="3">
@@ -1094,18 +1089,18 @@
       <c r="E16" s="3">
         <v>43080</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="3">
@@ -1114,18 +1109,18 @@
       <c r="E17" s="3">
         <v>43080</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="3">
@@ -1134,18 +1129,18 @@
       <c r="E18" s="3">
         <v>43081</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="17">
         <v>14</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="3">
@@ -1154,7 +1149,7 @@
       <c r="E19" s="3">
         <v>43082</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1190,37 +1185,37 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.19921875" customWidth="1"/>
-    <col min="3" max="3" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.19921875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="27" t="s">
         <v>55</v>
       </c>
@@ -1231,20 +1226,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="10" t="s">
+    <row r="2" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="28"/>
@@ -1252,13 +1247,13 @@
       <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="6">
@@ -1280,13 +1275,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="6">
@@ -1308,13 +1303,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="6">
@@ -1336,13 +1331,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="6">
@@ -1368,13 +1363,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="6">
@@ -1400,13 +1395,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="6">
@@ -1432,28 +1427,28 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>43076</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="8">
         <v>43076</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>43076</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>43076</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -1464,19 +1459,19 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>43073</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="8">
         <v>43073</v>
       </c>
       <c r="F10" s="4"/>
@@ -1492,19 +1487,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>43073</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>43073</v>
       </c>
       <c r="F11" s="4"/>
@@ -1519,20 +1514,20 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+    <row r="12" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>43073</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="8">
         <v>43073</v>
       </c>
       <c r="F12" s="4"/>
@@ -1548,19 +1543,19 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="23">
         <v>11</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="11">
-        <v>43075</v>
-      </c>
-      <c r="E13" s="11">
+      <c r="D13" s="8">
+        <v>43075</v>
+      </c>
+      <c r="E13" s="8">
         <v>43075</v>
       </c>
       <c r="F13" s="4"/>
@@ -1576,24 +1571,24 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="15">
         <v>12</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>43081</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="8">
         <v>43081</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I14" s="4" t="s">
@@ -1604,24 +1599,24 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="15">
         <v>13</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="8">
         <v>43081</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="8">
         <v>43081</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -1632,13 +1627,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="6">
@@ -1660,13 +1655,13 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="13" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="6">
@@ -1688,13 +1683,13 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="13" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="6">
@@ -1716,13 +1711,13 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+      <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="6">
@@ -1744,13 +1739,13 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
+      <c r="A20" s="23">
         <v>15</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="23" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1770,13 +1765,13 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="23">
         <v>16</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="23" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -1796,19 +1791,19 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
+      <c r="A22" s="23">
         <v>17</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="8">
         <v>43082</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="8">
         <v>43082</v>
       </c>
       <c r="F22" s="4"/>

</xml_diff>